<commit_message>
Update readme and matrix
</commit_message>
<xml_diff>
--- a/Lab1/Lab1.3 Matrix/Traceability Matrix.xlsx
+++ b/Lab1/Lab1.3 Matrix/Traceability Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\UIT\HK5\SE357\Đồ án\Lab1\Lab1.3 Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968416FD-2855-43A2-A177-7A08C3DBD5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05566F00-3E02-4E91-9E6B-8CF6963E72EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{01BCCBD6-42DA-4B8D-96FE-E09E808A3F6C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{01BCCBD6-42DA-4B8D-96FE-E09E808A3F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Linkable Traceability Matrix" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="56">
   <si>
     <t>Đăng nhập/Đăng ký</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Tìm kiếm</t>
-  </si>
-  <si>
-    <t>Truy cập</t>
   </si>
   <si>
     <t>Quản lý phân tích/thống kê</t>
@@ -194,13 +191,34 @@
   </si>
   <si>
     <t>Business standard</t>
+  </si>
+  <si>
+    <t>Truy cập thông tin cá nhân</t>
+  </si>
+  <si>
+    <t>Truy cập thông tin công ty</t>
+  </si>
+  <si>
+    <t>Req017</t>
+  </si>
+  <si>
+    <t>Quản lý tài khoản</t>
+  </si>
+  <si>
+    <t>Gợi ý việc làm</t>
+  </si>
+  <si>
+    <t>Req018</t>
+  </si>
+  <si>
+    <t>Req019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +251,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -273,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -296,7 +320,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5412A5-3154-4866-A3A8-949803F1AAE2}">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,62 +650,75 @@
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="10"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -693,17 +734,22 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="4"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -712,28 +758,34 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -744,21 +796,26 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -771,31 +828,37 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="4"/>
-      <c r="T5" s="5"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="4"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -803,25 +866,31 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="T6" s="5"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="4"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -835,18 +904,22 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="4"/>
-      <c r="T7" s="5"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="4"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -863,14 +936,18 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="T8" s="5"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="4"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -885,18 +962,22 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q9" s="4"/>
-      <c r="T9" s="5"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -913,14 +994,18 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="T10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="4"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -937,14 +1022,18 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="T11" s="5"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="4"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -957,17 +1046,21 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="T12" s="5"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="4"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -981,17 +1074,21 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="T13" s="5"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="4"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1009,15 +1106,17 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="T14" s="5"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="4"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>34</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1033,14 +1132,18 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-      <c r="T15" s="5"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="4"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1057,14 +1160,18 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="T16" s="5"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="4"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1081,55 +1188,163 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
-      <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="T18" s="5"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="T19" s="5"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="T20" s="5"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="T21" s="5"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R17" s="4"/>
+      <c r="S17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U17" s="3"/>
+      <c r="V17" s="4"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="4"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="4"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="4"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="4"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="U22" s="5"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
@@ -1140,14 +1355,17 @@
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1157,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBE8DA4-EBB5-400C-A8AA-1E9DD2F6C1BE}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A17"/>
+      <selection activeCell="A2" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,172 +1390,172 @@
   <sheetData>
     <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="9">
         <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="9">
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="9">
         <v>2</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="9">
         <v>4</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="9">
         <v>4</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="9">
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="9">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="9">
         <v>3</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="9">
         <v>4</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="9">
         <v>3</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="9">
         <v>3</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="9">
         <v>5</v>
@@ -1348,26 +1566,38 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="9">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="9">
+        <v>5</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBE09F3-F434-49CF-934B-4473CDE4976C}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1381,306 +1611,322 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>43</v>
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>43</v>
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>43</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>43</v>
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>43</v>
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>43</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>43</v>
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>43</v>
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>43</v>
+        <v>27</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>43</v>
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>43</v>
+        <v>29</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>43</v>
+        <v>30</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>43</v>
+        <v>31</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1690,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC33AC2-DBF5-49BF-BBB9-8D584AA49C9B}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B17"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1704,15 +1950,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1720,15 +1966,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -1736,7 +1982,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
@@ -1744,7 +1990,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -1752,7 +1998,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -1760,7 +2006,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
@@ -1768,7 +2014,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
@@ -1776,7 +2022,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -1784,7 +2030,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -1792,7 +2038,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
@@ -1800,7 +2046,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>10</v>
@@ -1808,35 +2054,63 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>